<commit_message>
EPBDS-7421 Don't skip evaluation of null values
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Arrays_transform.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Arrays_transform.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
@@ -10,7 +10,7 @@
     <sheet name="setUp" sheetId="1" r:id="rId1"/>
     <sheet name="Tests" sheetId="8" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="65">
   <si>
     <t xml:space="preserve">Datatype car </t>
   </si>
@@ -82,9 +82,6 @@
     <t>car10</t>
   </si>
   <si>
-    <t>return arr[*@ name + " - " + val];</t>
-  </si>
-  <si>
     <t>Method String[] transformTo(car[] arr)</t>
   </si>
   <si>
@@ -172,9 +169,6 @@
     <t>_res_[0]</t>
   </si>
   <si>
-    <t>car1 - 8</t>
-  </si>
-  <si>
     <t>1,2,3,4,5</t>
   </si>
   <si>
@@ -190,39 +184,6 @@
     <t>_res_[4]</t>
   </si>
   <si>
-    <t>car2 - 8</t>
-  </si>
-  <si>
-    <t>car3 - 8</t>
-  </si>
-  <si>
-    <t>car4 - null</t>
-  </si>
-  <si>
-    <t>car5 - 5</t>
-  </si>
-  <si>
-    <t>car1 - null</t>
-  </si>
-  <si>
-    <t>car2 - 1</t>
-  </si>
-  <si>
-    <t>car1 - 5</t>
-  </si>
-  <si>
-    <t>car2 - 5</t>
-  </si>
-  <si>
-    <t>car4 - 5</t>
-  </si>
-  <si>
-    <t>Method String[] transformToWithPredicate(car[] arr)</t>
-  </si>
-  <si>
-    <t>return arr[transform to name + " - " + val];</t>
-  </si>
-  <si>
     <t>Test transformToWithPredicate</t>
   </si>
   <si>
@@ -238,16 +199,28 @@
     <t>Method Integer[] transformToUniquePredicate(car[] arr)</t>
   </si>
   <si>
-    <t>return arr[transform unique to val];</t>
-  </si>
-  <si>
     <t>Test transformToUniquePredicate</t>
+  </si>
+  <si>
+    <t>return arr[*@ name];</t>
+  </si>
+  <si>
+    <t>Method Integer[] transformToWithPredicate(car[] arr)</t>
+  </si>
+  <si>
+    <t>return arr[(x) transform to isEmpty(x) ? -1 : val];</t>
+  </si>
+  <si>
+    <t>_res_[5]</t>
+  </si>
+  <si>
+    <t>return arr[(x) transform unique to isEmpty(x) ? -1 : val ];</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -265,7 +238,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -288,35 +261,23 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -586,7 +547,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -597,7 +558,7 @@
   <dimension ref="B5:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,10 +572,13 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="F5" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -623,6 +587,9 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -637,17 +604,21 @@
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F9" s="2"/>
+      <c r="F9" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F10" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="F11" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="B11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -662,9 +633,6 @@
       </c>
       <c r="D12" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -729,9 +697,6 @@
       <c r="D16" s="1">
         <v>8</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -745,9 +710,6 @@
         <v>13</v>
       </c>
       <c r="D17" s="1"/>
-      <c r="F17" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -812,7 +774,7 @@
         <v>8</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -830,7 +792,7 @@
         <v>9</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -853,7 +815,7 @@
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F24" s="1" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -862,7 +824,7 @@
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F25" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -971,10 +933,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:W58"/>
+  <dimension ref="B2:Y58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="K50" sqref="K50"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="W54" sqref="W54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,59 +959,61 @@
     <col min="18" max="18" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
-    </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="K3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+    </row>
+    <row r="4" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1057,131 +1021,143 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="K4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="T4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>10</v>
@@ -1203,22 +1179,23 @@
       <c r="S6" s="1">
         <v>5</v>
       </c>
-      <c r="T6" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="U6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="V6" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="W6" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1227,7 +1204,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="K7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>10</v>
@@ -1235,15 +1212,9 @@
       <c r="M7" s="1">
         <v>5</v>
       </c>
-      <c r="N7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O7" s="1">
-        <v>5</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
       <c r="Q7" s="1">
         <v>5</v>
       </c>
@@ -1253,25 +1224,23 @@
       <c r="S7" s="1">
         <v>5</v>
       </c>
-      <c r="T7" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="T7" s="1"/>
       <c r="U7" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1279,133 +1248,135 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1">
         <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="D12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="18" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="K19" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K19" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
-      <c r="U19" s="5"/>
-      <c r="V19" s="5"/>
-      <c r="W19" s="5"/>
-    </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+      <c r="X19" s="6"/>
+      <c r="Y19" s="6"/>
+    </row>
+    <row r="20" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1413,131 +1384,141 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="K20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="N20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="N20" s="1" t="s">
+      <c r="O20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="O20" s="1" t="s">
+      <c r="P20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P20" s="1" t="s">
+      <c r="Q20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Q20" s="1" t="s">
+      <c r="R20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="R20" s="1" t="s">
+      <c r="S20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="S20" s="1" t="s">
+      <c r="T20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y20" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y21" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="3">
+        <v>8</v>
+      </c>
+      <c r="E22" s="3">
+        <v>8</v>
+      </c>
+      <c r="F22" s="3">
+        <v>8</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3">
+        <v>5</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="T20" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="U20" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="V20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="W20" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q21" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="S21" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="T21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="U21" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="V21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="W21" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>10</v>
@@ -1559,22 +1540,24 @@
       <c r="S22" s="1">
         <v>5</v>
       </c>
-      <c r="T22" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="U22" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="V22" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="W22" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="T22">
+        <v>-1</v>
+      </c>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1">
+        <v>1</v>
+      </c>
+      <c r="W22" s="1">
+        <v>-1</v>
+      </c>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1583,7 +1566,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="K23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>10</v>
@@ -1609,25 +1592,31 @@
       <c r="S23" s="1">
         <v>5</v>
       </c>
-      <c r="T23" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="U23" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="V23" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="W23" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="T23" s="1">
+        <v>-1</v>
+      </c>
+      <c r="U23" s="1">
+        <v>5</v>
+      </c>
+      <c r="V23" s="1">
+        <v>5</v>
+      </c>
+      <c r="W23" s="1">
+        <v>-1</v>
+      </c>
+      <c r="X23" s="1">
+        <v>5</v>
+      </c>
+      <c r="Y23" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -1635,129 +1624,125 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C25" s="1">
         <v>4</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="3">
+        <v>8</v>
+      </c>
+      <c r="E26" s="3">
+        <v>8</v>
+      </c>
+      <c r="F26" s="3">
+        <v>8</v>
+      </c>
+      <c r="G26" s="3">
+        <v>8</v>
+      </c>
+      <c r="H26" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="3">
+        <v>8</v>
+      </c>
+      <c r="E28" s="3">
+        <v>8</v>
+      </c>
+      <c r="F28" s="3">
+        <v>8</v>
+      </c>
+      <c r="G28" s="3"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="33" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B33" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="33" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B33" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-    </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="F34" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
-      <c r="K34" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="L34" s="5"/>
-      <c r="M34" s="5"/>
-      <c r="N34" s="5"/>
-      <c r="O34" s="5"/>
-      <c r="P34" s="5"/>
-      <c r="Q34" s="5"/>
-      <c r="R34" s="5"/>
-      <c r="S34" s="5"/>
-      <c r="T34" s="5"/>
-      <c r="U34" s="5"/>
-      <c r="V34" s="5"/>
-      <c r="W34" s="7"/>
-    </row>
-    <row r="35" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="K34" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="6"/>
+      <c r="S34" s="6"/>
+      <c r="T34" s="6"/>
+      <c r="U34" s="6"/>
+      <c r="V34" s="6"/>
+      <c r="W34" s="6"/>
+      <c r="X34" s="6"/>
+      <c r="Y34" s="6"/>
+    </row>
+    <row r="35" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -1765,117 +1750,133 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="K35" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M35" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M35" s="1" t="s">
+      <c r="N35" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="N35" s="1" t="s">
+      <c r="O35" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="O35" s="1" t="s">
+      <c r="P35" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P35" s="1" t="s">
+      <c r="Q35" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Q35" s="1" t="s">
+      <c r="R35" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="R35" s="1" t="s">
+      <c r="S35" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="S35" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="T35" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="U35" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="V35" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W35" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="V35" s="1" t="s">
+      <c r="X35" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="W35" s="7"/>
-    </row>
-    <row r="36" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="Y35" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D36" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="K36" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M36" s="1" t="s">
+      <c r="N36" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="N36" s="1" t="s">
+      <c r="O36" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="O36" s="1" t="s">
+      <c r="P36" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P36" s="1" t="s">
+      <c r="Q36" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Q36" s="1" t="s">
+      <c r="R36" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="R36" s="1" t="s">
+      <c r="S36" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="S36" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="T36" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U36" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="V36" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W36" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X36" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y36" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="U36" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="V36" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="W36" s="7"/>
-    </row>
-    <row r="37" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B37" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="D37" s="3">
         <v>8</v>
       </c>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3">
-        <v>5</v>
-      </c>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
+      <c r="E37" s="3">
+        <v>5</v>
+      </c>
+      <c r="F37" s="3"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
       <c r="K37" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>10</v>
@@ -1897,18 +1898,20 @@
       <c r="S37" s="1">
         <v>5</v>
       </c>
-      <c r="T37" s="1"/>
+      <c r="T37">
+        <v>1</v>
+      </c>
       <c r="U37" s="1">
-        <v>1</v>
-      </c>
-      <c r="V37" s="3">
-        <v>5</v>
-      </c>
-      <c r="W37" s="7"/>
-    </row>
-    <row r="38" spans="2:23" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="V37" s="1"/>
+      <c r="W37" s="1"/>
+      <c r="X37" s="1"/>
+      <c r="Y37" s="1"/>
+    </row>
+    <row r="38" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -1917,7 +1920,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="K38" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L38" s="1" t="s">
         <v>10</v>
@@ -1948,14 +1951,16 @@
       </c>
       <c r="U38" s="1"/>
       <c r="V38" s="1"/>
-      <c r="W38" s="7"/>
-    </row>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+      <c r="Y38" s="1"/>
+    </row>
+    <row r="39" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -1963,9 +1968,9 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C40" s="1">
         <v>4</v>
@@ -1976,27 +1981,27 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="D41" s="3">
         <v>8</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-    </row>
-    <row r="42" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -2004,69 +2009,72 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="D43" s="3">
         <v>8</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
-      <c r="G43" s="6"/>
+      <c r="G43" s="4"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="48" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B48" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
-    </row>
-    <row r="49" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B48" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+    </row>
+    <row r="49" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="D49" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
-      <c r="K49" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="L49" s="5"/>
-      <c r="M49" s="5"/>
-      <c r="N49" s="5"/>
-      <c r="O49" s="5"/>
-      <c r="P49" s="5"/>
-      <c r="Q49" s="5"/>
-      <c r="R49" s="5"/>
-      <c r="S49" s="5"/>
-      <c r="T49" s="5"/>
-      <c r="U49" s="5"/>
-      <c r="V49" s="5"/>
-    </row>
-    <row r="50" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="K49" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="L49" s="6"/>
+      <c r="M49" s="6"/>
+      <c r="N49" s="6"/>
+      <c r="O49" s="6"/>
+      <c r="P49" s="6"/>
+      <c r="Q49" s="6"/>
+      <c r="R49" s="6"/>
+      <c r="S49" s="6"/>
+      <c r="T49" s="6"/>
+      <c r="U49" s="6"/>
+      <c r="V49" s="6"/>
+      <c r="W49" s="6"/>
+      <c r="X49" s="6"/>
+      <c r="Y49" s="6"/>
+    </row>
+    <row r="50" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -2074,115 +2082,133 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
       <c r="K50" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L50" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M50" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M50" s="1" t="s">
+      <c r="N50" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="N50" s="1" t="s">
+      <c r="O50" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="O50" s="1" t="s">
+      <c r="P50" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P50" s="1" t="s">
+      <c r="Q50" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Q50" s="1" t="s">
+      <c r="R50" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="R50" s="1" t="s">
+      <c r="S50" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="S50" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="T50" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="U50" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="V50" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W50" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="V50" s="1" t="s">
+      <c r="X50" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="51" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="Y50" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D51" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
       <c r="K51" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L51" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M51" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M51" s="1" t="s">
+      <c r="N51" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="N51" s="1" t="s">
+      <c r="O51" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="O51" s="1" t="s">
+      <c r="P51" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P51" s="1" t="s">
+      <c r="Q51" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Q51" s="1" t="s">
+      <c r="R51" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="R51" s="1" t="s">
+      <c r="S51" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="S51" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="T51" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U51" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="V51" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W51" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X51" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y51" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="U51" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="V51" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="52" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B52" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="D52" s="3">
         <v>8</v>
       </c>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3">
-        <v>5</v>
-      </c>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
+      <c r="E52" s="3">
+        <v>5</v>
+      </c>
+      <c r="F52" s="3"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
       <c r="K52" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L52" s="1" t="s">
         <v>10</v>
@@ -2204,17 +2230,22 @@
       <c r="S52" s="1">
         <v>5</v>
       </c>
-      <c r="T52" s="1"/>
+      <c r="T52">
+        <v>-1</v>
+      </c>
       <c r="U52" s="1">
         <v>1</v>
       </c>
-      <c r="V52" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="V52" s="1">
+        <v>5</v>
+      </c>
+      <c r="W52" s="1"/>
+      <c r="X52" s="1"/>
+      <c r="Y52" s="1"/>
+    </row>
+    <row r="53" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -2223,7 +2254,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
       <c r="K53" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L53" s="1" t="s">
         <v>10</v>
@@ -2250,17 +2281,22 @@
         <v>5</v>
       </c>
       <c r="T53" s="1">
-        <v>5</v>
-      </c>
-      <c r="U53" s="1"/>
+        <v>-1</v>
+      </c>
+      <c r="U53" s="1">
+        <v>5</v>
+      </c>
       <c r="V53" s="1"/>
-    </row>
-    <row r="54" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="W53" s="1"/>
+      <c r="X53" s="1"/>
+      <c r="Y53" s="1"/>
+    </row>
+    <row r="54" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -2268,9 +2304,9 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C55" s="1">
         <v>4</v>
@@ -2281,27 +2317,27 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="D56" s="3">
         <v>8</v>
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
-      <c r="G56" s="6"/>
-      <c r="H56" s="6"/>
-    </row>
-    <row r="57" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+    </row>
+    <row r="57" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -2309,31 +2345,31 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C58" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="D58" s="3">
         <v>8</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
-      <c r="G58" s="6"/>
+      <c r="G58" s="4"/>
       <c r="H58" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="K49:V49"/>
     <mergeCell ref="B33:F33"/>
-    <mergeCell ref="K34:V34"/>
     <mergeCell ref="B48:F48"/>
     <mergeCell ref="B2:H2"/>
-    <mergeCell ref="K3:W3"/>
     <mergeCell ref="B18:H18"/>
-    <mergeCell ref="K19:W19"/>
+    <mergeCell ref="K3:Y3"/>
+    <mergeCell ref="K19:Y19"/>
+    <mergeCell ref="K49:Y49"/>
+    <mergeCell ref="K34:Y34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
EPBDS-8047 Fix error on creation of array of primitives
--HG--
branch : 5.21.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Arrays_transform.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Arrays_transform.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="setUp" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="71">
   <si>
     <t xml:space="preserve">Datatype car </t>
   </si>
@@ -215,6 +215,24 @@
   </si>
   <si>
     <t>return arr[(x) transform unique to isEmpty(x) ? -1 : val ];</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>pos</t>
+  </si>
+  <si>
+    <t>return arr[(x) transform unique to isEmpty(x) ? -1 : pos ];</t>
+  </si>
+  <si>
+    <t>return arr[(x) transform to isEmpty(x) ? -1 : pos];</t>
+  </si>
+  <si>
+    <t>Method Integer[] transformToWithPredicate2(car[] arr)</t>
+  </si>
+  <si>
+    <t>Method Integer[] transformToUniquePredicate2(car[] arr)</t>
   </si>
 </sst>
 </file>
@@ -555,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:J38"/>
+  <dimension ref="B5:K38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,65 +584,73 @@
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="63.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" customWidth="1"/>
+    <col min="7" max="7" width="63.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="61.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="6"/>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F9" s="1" t="s">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G9" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F10" s="1" t="s">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G10" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
-      <c r="G11" s="2"/>
+      <c r="E11" s="6"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
@@ -634,12 +660,15 @@
       <c r="D12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="2"/>
+      <c r="E12" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
@@ -649,13 +678,16 @@
       <c r="D13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="E13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>1</v>
       </c>
@@ -665,13 +697,18 @@
       <c r="D14" s="1">
         <v>8</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>2</v>
       </c>
@@ -681,13 +718,16 @@
       <c r="D15" s="1">
         <v>8</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="E15" s="1">
+        <v>2</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>3</v>
       </c>
@@ -697,12 +737,15 @@
       <c r="D16" s="1">
         <v>8</v>
       </c>
-      <c r="G16" s="2"/>
+      <c r="E16" s="1">
+        <v>3</v>
+      </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>4</v>
       </c>
@@ -710,12 +753,15 @@
         <v>13</v>
       </c>
       <c r="D17" s="1"/>
-      <c r="G17" s="2"/>
+      <c r="E17" s="1">
+        <v>4</v>
+      </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>5</v>
       </c>
@@ -725,13 +771,16 @@
       <c r="D18" s="1">
         <v>5</v>
       </c>
-      <c r="F18" s="2"/>
+      <c r="E18" s="1">
+        <v>5</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>6</v>
       </c>
@@ -741,13 +790,16 @@
       <c r="D19" s="1">
         <v>6</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="E19" s="1">
+        <v>6</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>7</v>
       </c>
@@ -757,13 +809,16 @@
       <c r="D20" s="1">
         <v>7</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="E20" s="1">
+        <v>7</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>8</v>
       </c>
@@ -773,15 +828,18 @@
       <c r="D21" s="1">
         <v>8</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="E21" s="1">
+        <v>8</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>9</v>
       </c>
@@ -791,15 +849,18 @@
       <c r="D22" s="1">
         <v>9</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="E22" s="1">
+        <v>9</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>10</v>
       </c>
@@ -807,125 +868,132 @@
         <v>19</v>
       </c>
       <c r="D23" s="1"/>
-      <c r="F23" s="2"/>
+      <c r="E23" s="1">
+        <v>10</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F24" s="1" t="s">
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G24" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F25" s="1" t="s">
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F26" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F27" s="2"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G28" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G29" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F30" s="2"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F31" s="2"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F32" s="2"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
-    </row>
-    <row r="33" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F33" s="2"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
-    </row>
-    <row r="34" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F34" s="2"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
-    </row>
-    <row r="35" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F35" s="2"/>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
-    </row>
-    <row r="36" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F36" s="2"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
-    </row>
-    <row r="37" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F37" s="2"/>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
-    </row>
-    <row r="38" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F38" s="2"/>
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -935,8 +1003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Y58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="W54" sqref="W54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2362,14 +2430,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="K49:Y49"/>
+    <mergeCell ref="K34:Y34"/>
     <mergeCell ref="B33:F33"/>
     <mergeCell ref="B48:F48"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B18:H18"/>
     <mergeCell ref="K3:Y3"/>
     <mergeCell ref="K19:Y19"/>
-    <mergeCell ref="K49:Y49"/>
-    <mergeCell ref="K34:Y34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>